<commit_message>
re-classify vehicles and fit survival patterns
</commit_message>
<xml_diff>
--- a/data/Fuel Data 2022-2023-2024-2025 from all stations-2.xlsx
+++ b/data/Fuel Data 2022-2023-2024-2025 from all stations-2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C609209-ABA4-4045-BB9A-630BEE8D0C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460AA19B-683D-7E40-A60A-39B8160804C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34620" windowHeight="20640" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34620" windowHeight="14260" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Stations" sheetId="3" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All Stations'!$A$1:$F$43</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="191029" calcMode="manual" iterateDelta="1.0000000000000001E-5" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -537,8 +537,8 @@
         <v>6</v>
       </c>
       <c r="H2">
-        <f>SUM(B2:D13)</f>
-        <v>38194769</v>
+        <f>SUM(C2:D13)</f>
+        <v>28142475</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -772,9 +772,9 @@
       <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H14">
-        <f>SUM(B14:D25)</f>
-        <v>35619474</v>
+      <c r="H14" s="1">
+        <f>SUM(C14:D25)</f>
+        <v>29666405</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1009,8 +1009,8 @@
         <v>6</v>
       </c>
       <c r="H26" s="6">
-        <f>SUM(B26:D37)</f>
-        <v>37086643</v>
+        <f>SUM(C26:D37)</f>
+        <v>31897882</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1360,9 +1360,6 @@
     <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K000000&amp;1#</oddHeader>
     <oddFooter>&amp;L&amp;1#&amp;"Arial"&amp;10&amp;K000000Saudi Aramco: Company General Use</oddFooter>
   </headerFooter>
-  <ignoredErrors>
-    <ignoredError sqref="H2"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>